<commit_message>
edit file  data definition
</commit_message>
<xml_diff>
--- a/documentation/Kitkot_data_definition.xlsx
+++ b/documentation/Kitkot_data_definition.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\29532\Desktop\Kitkot\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P\Desktop\projet\Kitkot\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8630AE-21AD-4422-9AFB-004FD4E4B736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E572E699-F669-4221-AB19-EDF9B8DED606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{74DD5BA1-0DD9-41A3-84E5-D6BD4BE7C3AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{74DD5BA1-0DD9-41A3-84E5-D6BD4BE7C3AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>USERS</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t xml:space="preserve">                                                          KITKOT DATA DEFINITION</t>
+  </si>
+  <si>
+    <t>indenfiant utilisateur</t>
   </si>
 </sst>
 </file>
@@ -198,22 +201,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -221,6 +217,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -539,82 +538,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EE0CF0-98D5-4DE0-B321-4A4221CF3977}">
   <dimension ref="A2:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -627,11 +621,13 @@
       <c r="D8" s="1">
         <v>50</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -646,7 +642,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -662,7 +658,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -672,14 +668,14 @@
       <c r="C11" s="1">
         <v>50</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -695,7 +691,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -703,7 +699,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -711,7 +707,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -719,7 +715,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -727,7 +723,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -735,35 +731,35 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -779,8 +775,8 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -795,7 +791,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -813,7 +809,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
@@ -829,7 +825,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -845,7 +841,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -861,7 +857,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -877,7 +873,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -893,7 +889,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
@@ -909,7 +905,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -917,7 +913,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -925,35 +921,35 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
@@ -969,8 +965,8 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -983,7 +979,7 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>11</v>
       </c>
@@ -999,7 +995,7 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>12</v>
       </c>
@@ -1015,7 +1011,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1023,7 +1019,7 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>

</xml_diff>